<commit_message>
Bulk Upload, loan counts
Bulk upload updated with closed status.
Bulk upload format file also updated.
Loan count reworked to get exact count.
</commit_message>
<xml_diff>
--- a/uploads/excel_format/bulk upload format.xlsx
+++ b/uploads/excel_format/bulk upload format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Marudham\uploads\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="142">
   <si>
     <t>Sl.no</t>
   </si>
@@ -377,12 +377,6 @@
     <t>Resident</t>
   </si>
   <si>
-    <t>G D</t>
-  </si>
-  <si>
-    <t>L D</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -426,6 +420,36 @@
   </si>
   <si>
     <t>P Ramarajan</t>
+  </si>
+  <si>
+    <t>Closed Status</t>
+  </si>
+  <si>
+    <t>Consider Level</t>
+  </si>
+  <si>
+    <t>Closed Remark</t>
+  </si>
+  <si>
+    <t>Consider</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Closed Date</t>
+  </si>
+  <si>
+    <t>Raguvaran</t>
+  </si>
+  <si>
+    <t>GD1</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -779,11 +803,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CO13"/>
+  <dimension ref="A1:CS13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CO1" sqref="CO1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -878,9 +900,12 @@
     <col min="91" max="91" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="95" max="96" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:97" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1160,8 +1185,20 @@
       <c r="CO1" s="9" t="s">
         <v>91</v>
       </c>
+      <c r="CP1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="CQ1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="CR1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="CS1" s="9" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1169,14 +1206,14 @@
         <v>45238</v>
       </c>
       <c r="C2" s="3">
-        <v>239903777436</v>
+        <v>271232712327</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G2" s="2">
         <v>32874</v>
@@ -1203,10 +1240,10 @@
         <v>97</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P2" s="1">
-        <v>9092878519</v>
+        <v>2712327123</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>98</v>
@@ -1221,7 +1258,7 @@
         <v>101</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>102</v>
@@ -1310,7 +1347,7 @@
         <v>112</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>113</v>
@@ -1325,31 +1362,31 @@
         <v>116</v>
       </c>
       <c r="BE2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="BG2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="BF2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="BH2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="BI2" s="2">
         <v>45238</v>
       </c>
       <c r="BJ2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="BL2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BM2" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="BN2" s="4"/>
       <c r="BO2" s="4"/>
@@ -1396,28 +1433,28 @@
         <v>45422</v>
       </c>
       <c r="CD2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="CE2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="CF2" s="3">
         <v>239903777436</v>
       </c>
       <c r="CG2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CH2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="CI2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="CH2" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="CI2" s="6" t="s">
+      <c r="CK2" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="CL2" s="7">
         <v>14700</v>
@@ -1429,10 +1466,22 @@
         <v>239903777436</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>136</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CS2" s="2">
+        <v>45483</v>
       </c>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1522,7 +1571,7 @@
       <c r="CN3" s="3"/>
       <c r="CO3" s="1"/>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1612,7 +1661,7 @@
       <c r="CN4" s="3"/>
       <c r="CO4" s="1"/>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -1702,7 +1751,7 @@
       <c r="CN5" s="3"/>
       <c r="CO5" s="1"/>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
@@ -1791,7 +1840,7 @@
       <c r="CN6" s="3"/>
       <c r="CO6" s="1"/>
     </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
@@ -1880,7 +1929,7 @@
       <c r="CN7" s="3"/>
       <c r="CO7" s="1"/>
     </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -1969,7 +2018,7 @@
       <c r="CN8" s="3"/>
       <c r="CO8" s="1"/>
     </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -2058,7 +2107,7 @@
       <c r="CN9" s="3"/>
       <c r="CO9" s="1"/>
     </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -2148,7 +2197,7 @@
       <c r="CN10" s="3"/>
       <c r="CO10" s="1"/>
     </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -2238,7 +2287,7 @@
       <c r="CN11" s="3"/>
       <c r="CO11" s="1"/>
     </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -2328,7 +2377,7 @@
       <c r="CN12" s="3"/>
       <c r="CO12" s="1"/>
     </row>
-    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -2420,5 +2469,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>